<commit_message>
- Updated to reflect work done
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@2232 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-09 DSTU/QA/FMG QA Summary - outstanding issues.xlsx
+++ b/ballots/2013-09 DSTU/QA/FMG QA Summary - outstanding issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1605" windowWidth="29040" windowHeight="15405" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="1605" windowWidth="29040" windowHeight="15405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="For future consideration" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="141">
   <si>
     <t xml:space="preserve"> Basic Messaging Assumptions</t>
   </si>
@@ -308,12 +308,6 @@
     <t>The "values" element does not exist (anymore)</t>
   </si>
   <si>
-    <t>todo: fill out.</t>
-  </si>
-  <si>
-    <t>I think this is now done in the extensibility-examples page (in 1.11.6.1.1.5 to be exactly), so could refer to that.</t>
-  </si>
-  <si>
     <t>extensibility-examples.html</t>
   </si>
   <si>
@@ -369,51 +363,6 @@
     <t>It's not allowed as a data type, but it's a valid point. Revisit this in the future</t>
   </si>
   <si>
-    <r>
-      <t>TypeRef.code is from a fixed codeset, yet the profile example (profiles-resources.xml.html) sometimes uses </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>`ResourceReference(A|B|C)`</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> to specify the kind of ResourceReference allowed. This cannot be correct (since only </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>`ResourceReference`</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> is allowed as a code), and the allowed resource types should be split apart. </t>
-    </r>
-  </si>
-  <si>
     <t>The example lipid profile and the ones below this profile are rendered as raw XML whereas the first few are rendered in HTML (showing formatted XML) </t>
   </si>
   <si>
@@ -444,17 +393,6 @@
     <t>Much more complicated that it sounds unless we want to require UCUM. Not broken, so defer to future</t>
   </si>
   <si>
-    <t xml:space="preserve">There is a problem in the graphical rendering of resources.  The data within the box for a resource wraps incorrectly if the Resourc(A|B|C|D) causes a line wrap.  In particular, the first line ends in "|)" and then the next, indented line ends in ")"  There should be no ")" at end of first line.  I noticed this in:
-DocumentManifest (Resource)
-masterIdentifier : Identifier 1..1
-identifier : Identifier 0..*
-subject : Resource(Patient|Practitioner|Group|)
-       Device) 1..*
-recipient : Resource(Patient|Practitioner|)
-       Organization) 0..*
-type : CodeableConcept 0..1 </t>
-  </si>
-  <si>
     <t>Composition.instant should be a dateTime.  When converting from CDA, most will be dates, not timestamps.</t>
   </si>
   <si>
@@ -471,9 +409,6 @@
   </si>
   <si>
     <t>I agree. Can have a fax and a phone</t>
-  </si>
-  <si>
-    <t>Need to clarify that Document/_search always returns a feed of atom feeds (and ensure that the atom description (XML and JSON) and schema support this.</t>
   </si>
   <si>
     <t>If the value of the parameter is a number (potentially with &lt; etc), it is a search on the value (todo: units, canonical?)</t>
@@ -1217,16 +1152,16 @@
         <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1234,13 +1169,13 @@
         <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -1248,16 +1183,16 @@
         <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1265,44 +1200,44 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1250,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
@@ -1357,10 +1292,10 @@
         <v>42</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -1380,10 +1315,10 @@
         <v>43</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="150" hidden="1" x14ac:dyDescent="0.25">
@@ -1406,10 +1341,10 @@
         <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="210" hidden="1" x14ac:dyDescent="0.25">
@@ -1426,13 +1361,13 @@
         <v>46</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -1453,13 +1388,13 @@
         <v>49</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -1483,10 +1418,10 @@
         <v>54</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="165" hidden="1" x14ac:dyDescent="0.25">
@@ -1509,10 +1444,10 @@
         <v>61</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1531,55 +1466,55 @@
         <v>71</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="195" hidden="1" x14ac:dyDescent="0.25">
@@ -1605,31 +1540,31 @@
         <v>70</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1">
         <v>207</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1650,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,38 +1620,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>